<commit_message>
set types and requirements
</commit_message>
<xml_diff>
--- a/data/cohort-dataset-with-logreg-output.xlsx
+++ b/data/cohort-dataset-with-logreg-output.xlsx
@@ -983,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.786352276802063</v>
+        <v>0.7837604284286499</v>
       </c>
     </row>
     <row r="3">
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.8064717650413513</v>
+        <v>0.7279143333435059</v>
       </c>
     </row>
     <row r="4">
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.7285342216491699</v>
+        <v>0.813188374042511</v>
       </c>
     </row>
     <row r="5">
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.68931645154953</v>
+        <v>0.876110315322876</v>
       </c>
     </row>
     <row r="6">
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="BO6" t="n">
-        <v>0.7594887614250183</v>
+        <v>0.741787314414978</v>
       </c>
     </row>
     <row r="7">
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="BO7" t="n">
-        <v>0.6233391761779785</v>
+        <v>0.7662057876586914</v>
       </c>
     </row>
     <row r="8">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.7269136905670166</v>
+        <v>0.7803550958633423</v>
       </c>
     </row>
     <row r="9">
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.7122393846511841</v>
+        <v>0.7516946196556091</v>
       </c>
     </row>
     <row r="10">
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="BO10" t="n">
-        <v>0.7101767659187317</v>
+        <v>0.7472559809684753</v>
       </c>
     </row>
     <row r="11">
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="BO11" t="n">
-        <v>0.6924245953559875</v>
+        <v>0.7001696825027466</v>
       </c>
     </row>
     <row r="12">
@@ -3193,7 +3193,7 @@
         <v>0</v>
       </c>
       <c r="BO12" t="n">
-        <v>0.7626952528953552</v>
+        <v>0.7348120212554932</v>
       </c>
     </row>
     <row r="13">
@@ -3414,7 +3414,7 @@
         <v>0</v>
       </c>
       <c r="BO13" t="n">
-        <v>0.6768442988395691</v>
+        <v>0.7973758578300476</v>
       </c>
     </row>
     <row r="14">
@@ -3635,7 +3635,7 @@
         <v>0</v>
       </c>
       <c r="BO14" t="n">
-        <v>0.7537519335746765</v>
+        <v>0.7539451122283936</v>
       </c>
     </row>
     <row r="15">
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="BO15" t="n">
-        <v>0.5767948627471924</v>
+        <v>0.7015854716300964</v>
       </c>
     </row>
     <row r="16">
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
       <c r="BO16" t="n">
-        <v>0.7184497117996216</v>
+        <v>0.7444555759429932</v>
       </c>
     </row>
     <row r="17">
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="BO17" t="n">
-        <v>0.7840759754180908</v>
+        <v>0.7379483580589294</v>
       </c>
     </row>
     <row r="18">
@@ -4519,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="BO18" t="n">
-        <v>0.6821249127388</v>
+        <v>0.7753097414970398</v>
       </c>
     </row>
     <row r="19">
@@ -4740,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="BO19" t="n">
-        <v>0.4449077844619751</v>
+        <v>0.4195190370082855</v>
       </c>
     </row>
     <row r="20">
@@ -4961,7 +4961,7 @@
         <v>0</v>
       </c>
       <c r="BO20" t="n">
-        <v>0.7651219964027405</v>
+        <v>0.8011788129806519</v>
       </c>
     </row>
     <row r="21">
@@ -5182,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="BO21" t="n">
-        <v>0.5050538182258606</v>
+        <v>0.456044465303421</v>
       </c>
     </row>
     <row r="22">
@@ -5403,7 +5403,7 @@
         <v>0</v>
       </c>
       <c r="BO22" t="n">
-        <v>0.4140296280384064</v>
+        <v>0.5989366769790649</v>
       </c>
     </row>
     <row r="23">
@@ -5624,7 +5624,7 @@
         <v>0.395</v>
       </c>
       <c r="BO23" t="n">
-        <v>0.6882056593894958</v>
+        <v>0.7619568705558777</v>
       </c>
     </row>
     <row r="24">
@@ -5845,7 +5845,7 @@
         <v>0</v>
       </c>
       <c r="BO24" t="n">
-        <v>0.7019598484039307</v>
+        <v>0.7488059401512146</v>
       </c>
     </row>
     <row r="25">
@@ -6066,7 +6066,7 @@
         <v>0</v>
       </c>
       <c r="BO25" t="n">
-        <v>0.69632488489151</v>
+        <v>0.6251933574676514</v>
       </c>
     </row>
     <row r="26">
@@ -6287,7 +6287,7 @@
         <v>0</v>
       </c>
       <c r="BO26" t="n">
-        <v>0.8021796345710754</v>
+        <v>0.7168236970901489</v>
       </c>
     </row>
     <row r="27">
@@ -6508,7 +6508,7 @@
         <v>0.11</v>
       </c>
       <c r="BO27" t="n">
-        <v>0.6810404658317566</v>
+        <v>0.64058518409729</v>
       </c>
     </row>
     <row r="28">
@@ -6729,7 +6729,7 @@
         <v>0</v>
       </c>
       <c r="BO28" t="n">
-        <v>0.7579781413078308</v>
+        <v>0.8037018179893494</v>
       </c>
     </row>
     <row r="29">
@@ -6950,7 +6950,7 @@
         <v>0</v>
       </c>
       <c r="BO29" t="n">
-        <v>0.7118949294090271</v>
+        <v>0.625207245349884</v>
       </c>
     </row>
     <row r="30">
@@ -7171,7 +7171,7 @@
         <v>0</v>
       </c>
       <c r="BO30" t="n">
-        <v>0.7683327198028564</v>
+        <v>0.8132553100585938</v>
       </c>
     </row>
     <row r="31">
@@ -7392,7 +7392,7 @@
         <v>0</v>
       </c>
       <c r="BO31" t="n">
-        <v>0.6344376802444458</v>
+        <v>0.7647276520729065</v>
       </c>
     </row>
     <row r="32">
@@ -7613,7 +7613,7 @@
         <v>0</v>
       </c>
       <c r="BO32" t="n">
-        <v>0.7241398096084595</v>
+        <v>0.7053089737892151</v>
       </c>
     </row>
     <row r="33">
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
       <c r="BO33" t="n">
-        <v>0.6483899354934692</v>
+        <v>0.7426403760910034</v>
       </c>
     </row>
     <row r="34">
@@ -8055,7 +8055,7 @@
         <v>0</v>
       </c>
       <c r="BO34" t="n">
-        <v>0.5541936159133911</v>
+        <v>0.592975378036499</v>
       </c>
     </row>
     <row r="35">
@@ -8276,7 +8276,7 @@
         <v>0</v>
       </c>
       <c r="BO35" t="n">
-        <v>0.8008582592010498</v>
+        <v>0.7315511107444763</v>
       </c>
     </row>
     <row r="36">
@@ -8497,7 +8497,7 @@
         <v>0.132</v>
       </c>
       <c r="BO36" t="n">
-        <v>0.5578319430351257</v>
+        <v>0.5152532458305359</v>
       </c>
     </row>
     <row r="37">
@@ -8718,7 +8718,7 @@
         <v>0</v>
       </c>
       <c r="BO37" t="n">
-        <v>0.8166211843490601</v>
+        <v>0.7740731835365295</v>
       </c>
     </row>
     <row r="38">
@@ -8939,7 +8939,7 @@
         <v>0</v>
       </c>
       <c r="BO38" t="n">
-        <v>0.7163727283477783</v>
+        <v>0.7825538516044617</v>
       </c>
     </row>
     <row r="39">
@@ -9160,7 +9160,7 @@
         <v>0</v>
       </c>
       <c r="BO39" t="n">
-        <v>0.5754212737083435</v>
+        <v>0.462871640920639</v>
       </c>
     </row>
     <row r="40">
@@ -9381,7 +9381,7 @@
         <v>0</v>
       </c>
       <c r="BO40" t="n">
-        <v>0.6220903992652893</v>
+        <v>0.6657180786132812</v>
       </c>
     </row>
     <row r="41">
@@ -9602,7 +9602,7 @@
         <v>0</v>
       </c>
       <c r="BO41" t="n">
-        <v>0.5860722661018372</v>
+        <v>0.5833063125610352</v>
       </c>
     </row>
     <row r="42">
@@ -9823,7 +9823,7 @@
         <v>0</v>
       </c>
       <c r="BO42" t="n">
-        <v>0.4326642155647278</v>
+        <v>0.4351317882537842</v>
       </c>
     </row>
     <row r="43">
@@ -10044,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="BO43" t="n">
-        <v>0.5216021537780762</v>
+        <v>0.5796887874603271</v>
       </c>
     </row>
     <row r="44">
@@ -10265,7 +10265,7 @@
         <v>0</v>
       </c>
       <c r="BO44" t="n">
-        <v>0.7479337453842163</v>
+        <v>0.6429891586303711</v>
       </c>
     </row>
     <row r="45">
@@ -10486,7 +10486,7 @@
         <v>0</v>
       </c>
       <c r="BO45" t="n">
-        <v>0.3722509443759918</v>
+        <v>0.5113218426704407</v>
       </c>
     </row>
     <row r="46">
@@ -10707,7 +10707,7 @@
         <v>0</v>
       </c>
       <c r="BO46" t="n">
-        <v>0.3086816668510437</v>
+        <v>0.5236095190048218</v>
       </c>
     </row>
     <row r="47">
@@ -10928,7 +10928,7 @@
         <v>0</v>
       </c>
       <c r="BO47" t="n">
-        <v>0.7379691004753113</v>
+        <v>0.8046386241912842</v>
       </c>
     </row>
     <row r="48">
@@ -11149,7 +11149,7 @@
         <v>0</v>
       </c>
       <c r="BO48" t="n">
-        <v>0.7753419876098633</v>
+        <v>0.8060837388038635</v>
       </c>
     </row>
     <row r="49">
@@ -11370,7 +11370,7 @@
         <v>0</v>
       </c>
       <c r="BO49" t="n">
-        <v>0.7052682638168335</v>
+        <v>0.7836665511131287</v>
       </c>
     </row>
     <row r="50">
@@ -11591,7 +11591,7 @@
         <v>0</v>
       </c>
       <c r="BO50" t="n">
-        <v>0.698710024356842</v>
+        <v>0.7159928679466248</v>
       </c>
     </row>
     <row r="51">
@@ -11812,7 +11812,7 @@
         <v>0</v>
       </c>
       <c r="BO51" t="n">
-        <v>0.7692790031433105</v>
+        <v>0.7895399928092957</v>
       </c>
     </row>
     <row r="52">
@@ -12033,7 +12033,7 @@
         <v>0</v>
       </c>
       <c r="BO52" t="n">
-        <v>0.335590273141861</v>
+        <v>0.4180402159690857</v>
       </c>
     </row>
     <row r="53">
@@ -12254,7 +12254,7 @@
         <v>0</v>
       </c>
       <c r="BO53" t="n">
-        <v>0.2500689029693604</v>
+        <v>0.2976245582103729</v>
       </c>
     </row>
     <row r="54">
@@ -12475,7 +12475,7 @@
         <v>0</v>
       </c>
       <c r="BO54" t="n">
-        <v>0.005247752647846937</v>
+        <v>0.01408990658819675</v>
       </c>
     </row>
     <row r="55">
@@ -12696,7 +12696,7 @@
         <v>0</v>
       </c>
       <c r="BO55" t="n">
-        <v>0.6343542337417603</v>
+        <v>0.7957469820976257</v>
       </c>
     </row>
     <row r="56">
@@ -12917,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="BO56" t="n">
-        <v>0.7547188997268677</v>
+        <v>0.8261958956718445</v>
       </c>
     </row>
     <row r="57">
@@ -13138,7 +13138,7 @@
         <v>0</v>
       </c>
       <c r="BO57" t="n">
-        <v>0.7967960238456726</v>
+        <v>0.8513769507408142</v>
       </c>
     </row>
     <row r="58">
@@ -13359,7 +13359,7 @@
         <v>0.219</v>
       </c>
       <c r="BO58" t="n">
-        <v>0.8227890729904175</v>
+        <v>0.8695443868637085</v>
       </c>
     </row>
     <row r="59">
@@ -13580,7 +13580,7 @@
         <v>0</v>
       </c>
       <c r="BO59" t="n">
-        <v>0.7100624442100525</v>
+        <v>0.8374533653259277</v>
       </c>
     </row>
     <row r="60">
@@ -13801,7 +13801,7 @@
         <v>0.094</v>
       </c>
       <c r="BO60" t="n">
-        <v>0.7995694875717163</v>
+        <v>0.7939706444740295</v>
       </c>
     </row>
     <row r="61">
@@ -14022,7 +14022,7 @@
         <v>0</v>
       </c>
       <c r="BO61" t="n">
-        <v>0.7436298131942749</v>
+        <v>0.8358448147773743</v>
       </c>
     </row>
     <row r="62">
@@ -14243,7 +14243,7 @@
         <v>0</v>
       </c>
       <c r="BO62" t="n">
-        <v>0.7024329900741577</v>
+        <v>0.7842193245887756</v>
       </c>
     </row>
     <row r="63">
@@ -14464,7 +14464,7 @@
         <v>0</v>
       </c>
       <c r="BO63" t="n">
-        <v>0.6078312993049622</v>
+        <v>0.7223101258277893</v>
       </c>
     </row>
     <row r="64">
@@ -14685,7 +14685,7 @@
         <v>0</v>
       </c>
       <c r="BO64" t="n">
-        <v>0.6284248232841492</v>
+        <v>0.5808306932449341</v>
       </c>
     </row>
     <row r="65">
@@ -14906,7 +14906,7 @@
         <v>0</v>
       </c>
       <c r="BO65" t="n">
-        <v>0.681254506111145</v>
+        <v>0.6600769758224487</v>
       </c>
     </row>
     <row r="66">
@@ -15127,7 +15127,7 @@
         <v>0.073</v>
       </c>
       <c r="BO66" t="n">
-        <v>0.0925690084695816</v>
+        <v>0.145443394780159</v>
       </c>
     </row>
     <row r="67">
@@ -15348,7 +15348,7 @@
         <v>0</v>
       </c>
       <c r="BO67" t="n">
-        <v>0.6164453625679016</v>
+        <v>0.5602331757545471</v>
       </c>
     </row>
     <row r="68">
@@ -15569,7 +15569,7 @@
         <v>0</v>
       </c>
       <c r="BO68" t="n">
-        <v>0.1807530522346497</v>
+        <v>0.1382258832454681</v>
       </c>
     </row>
     <row r="69">
@@ -15790,7 +15790,7 @@
         <v>0</v>
       </c>
       <c r="BO69" t="n">
-        <v>0.742563784122467</v>
+        <v>0.7583444714546204</v>
       </c>
     </row>
     <row r="70">
@@ -16011,7 +16011,7 @@
         <v>0</v>
       </c>
       <c r="BO70" t="n">
-        <v>0.7599703073501587</v>
+        <v>0.6827608942985535</v>
       </c>
     </row>
     <row r="71">
@@ -16232,7 +16232,7 @@
         <v>0</v>
       </c>
       <c r="BO71" t="n">
-        <v>0.3593957722187042</v>
+        <v>0.3233097195625305</v>
       </c>
     </row>
     <row r="72">
@@ -16453,7 +16453,7 @@
         <v>0</v>
       </c>
       <c r="BO72" t="n">
-        <v>0.7051018476486206</v>
+        <v>0.7946881651878357</v>
       </c>
     </row>
     <row r="73">
@@ -16674,7 +16674,7 @@
         <v>0</v>
       </c>
       <c r="BO73" t="n">
-        <v>0.7297420501708984</v>
+        <v>0.7534769177436829</v>
       </c>
     </row>
     <row r="74">
@@ -16895,7 +16895,7 @@
         <v>0</v>
       </c>
       <c r="BO74" t="n">
-        <v>0.7228110432624817</v>
+        <v>0.7075704336166382</v>
       </c>
     </row>
     <row r="75">
@@ -17116,7 +17116,7 @@
         <v>0</v>
       </c>
       <c r="BO75" t="n">
-        <v>0.7849467992782593</v>
+        <v>0.8701086640357971</v>
       </c>
     </row>
     <row r="76">
@@ -17337,7 +17337,7 @@
         <v>0</v>
       </c>
       <c r="BO76" t="n">
-        <v>0.8017110228538513</v>
+        <v>0.821523129940033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add hyper-params optimization, requirements with versio
</commit_message>
<xml_diff>
--- a/data/cohort-dataset-with-logreg-output.xlsx
+++ b/data/cohort-dataset-with-logreg-output.xlsx
@@ -983,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.801789402961731</v>
+        <v>0.7066429257392883</v>
       </c>
     </row>
     <row r="3">
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.7560439109802246</v>
+        <v>0.8333324790000916</v>
       </c>
     </row>
     <row r="4">
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.6801273822784424</v>
+        <v>0.6847591996192932</v>
       </c>
     </row>
     <row r="5">
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.7160243391990662</v>
+        <v>0.7155214548110962</v>
       </c>
     </row>
     <row r="6">
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="BO6" t="n">
-        <v>0.6360751390457153</v>
+        <v>0.7534450888633728</v>
       </c>
     </row>
     <row r="7">
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="BO7" t="n">
-        <v>0.6878743171691895</v>
+        <v>0.6875506043434143</v>
       </c>
     </row>
     <row r="8">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.8232730031013489</v>
+        <v>0.7220718860626221</v>
       </c>
     </row>
     <row r="9">
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.7084152102470398</v>
+        <v>0.7777664661407471</v>
       </c>
     </row>
     <row r="10">
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="BO10" t="n">
-        <v>0.8131861686706543</v>
+        <v>0.8194712996482849</v>
       </c>
     </row>
     <row r="11">
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="BO11" t="n">
-        <v>0.7332450747489929</v>
+        <v>0.738487184047699</v>
       </c>
     </row>
     <row r="12">
@@ -3193,7 +3193,7 @@
         <v>0</v>
       </c>
       <c r="BO12" t="n">
-        <v>0.7843515872955322</v>
+        <v>0.6883087754249573</v>
       </c>
     </row>
     <row r="13">
@@ -3414,7 +3414,7 @@
         <v>0</v>
       </c>
       <c r="BO13" t="n">
-        <v>0.7271228432655334</v>
+        <v>0.759907066822052</v>
       </c>
     </row>
     <row r="14">
@@ -3635,7 +3635,7 @@
         <v>0</v>
       </c>
       <c r="BO14" t="n">
-        <v>0.8118029236793518</v>
+        <v>0.7971763610839844</v>
       </c>
     </row>
     <row r="15">
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="BO15" t="n">
-        <v>0.66534823179245</v>
+        <v>0.6778339147567749</v>
       </c>
     </row>
     <row r="16">
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
       <c r="BO16" t="n">
-        <v>0.7713174819946289</v>
+        <v>0.8134178519248962</v>
       </c>
     </row>
     <row r="17">
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="BO17" t="n">
-        <v>0.8052585124969482</v>
+        <v>0.6895470023155212</v>
       </c>
     </row>
     <row r="18">
@@ -4519,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="BO18" t="n">
-        <v>0.739811897277832</v>
+        <v>0.7083225846290588</v>
       </c>
     </row>
     <row r="19">
@@ -4740,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="BO19" t="n">
-        <v>0.1494527459144592</v>
+        <v>0.03088539279997349</v>
       </c>
     </row>
     <row r="20">
@@ -4961,7 +4961,7 @@
         <v>0</v>
       </c>
       <c r="BO20" t="n">
-        <v>0.7210519313812256</v>
+        <v>0.6962499022483826</v>
       </c>
     </row>
     <row r="21">
@@ -5182,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="BO21" t="n">
-        <v>0.267394632101059</v>
+        <v>0.2887141704559326</v>
       </c>
     </row>
     <row r="22">
@@ -5403,7 +5403,7 @@
         <v>0</v>
       </c>
       <c r="BO22" t="n">
-        <v>0.3803409934043884</v>
+        <v>0.4580791890621185</v>
       </c>
     </row>
     <row r="23">
@@ -5624,7 +5624,7 @@
         <v>0.395</v>
       </c>
       <c r="BO23" t="n">
-        <v>0.7185148000717163</v>
+        <v>0.7294402122497559</v>
       </c>
     </row>
     <row r="24">
@@ -5845,7 +5845,7 @@
         <v>0</v>
       </c>
       <c r="BO24" t="n">
-        <v>0.7936076521873474</v>
+        <v>0.6696252226829529</v>
       </c>
     </row>
     <row r="25">
@@ -6066,7 +6066,7 @@
         <v>0</v>
       </c>
       <c r="BO25" t="n">
-        <v>0.6275844573974609</v>
+        <v>0.6971911191940308</v>
       </c>
     </row>
     <row r="26">
@@ -6287,7 +6287,7 @@
         <v>0</v>
       </c>
       <c r="BO26" t="n">
-        <v>0.8039584755897522</v>
+        <v>0.7828356623649597</v>
       </c>
     </row>
     <row r="27">
@@ -6508,7 +6508,7 @@
         <v>0.11</v>
       </c>
       <c r="BO27" t="n">
-        <v>0.7431354522705078</v>
+        <v>0.6579923033714294</v>
       </c>
     </row>
     <row r="28">
@@ -6729,7 +6729,7 @@
         <v>0</v>
       </c>
       <c r="BO28" t="n">
-        <v>0.6699174046516418</v>
+        <v>0.6283414959907532</v>
       </c>
     </row>
     <row r="29">
@@ -6950,7 +6950,7 @@
         <v>0</v>
       </c>
       <c r="BO29" t="n">
-        <v>0.7253462672233582</v>
+        <v>0.6178016066551208</v>
       </c>
     </row>
     <row r="30">
@@ -7171,7 +7171,7 @@
         <v>0</v>
       </c>
       <c r="BO30" t="n">
-        <v>0.775775671005249</v>
+        <v>0.6607226729393005</v>
       </c>
     </row>
     <row r="31">
@@ -7392,7 +7392,7 @@
         <v>0</v>
       </c>
       <c r="BO31" t="n">
-        <v>0.7418695688247681</v>
+        <v>0.773419201374054</v>
       </c>
     </row>
     <row r="32">
@@ -7613,7 +7613,7 @@
         <v>0</v>
       </c>
       <c r="BO32" t="n">
-        <v>0.6562760472297668</v>
+        <v>0.6031879186630249</v>
       </c>
     </row>
     <row r="33">
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
       <c r="BO33" t="n">
-        <v>0.6888878345489502</v>
+        <v>0.5983608365058899</v>
       </c>
     </row>
     <row r="34">
@@ -8055,7 +8055,7 @@
         <v>0</v>
       </c>
       <c r="BO34" t="n">
-        <v>0.7161889672279358</v>
+        <v>0.701208233833313</v>
       </c>
     </row>
     <row r="35">
@@ -8276,7 +8276,7 @@
         <v>0</v>
       </c>
       <c r="BO35" t="n">
-        <v>0.7166765928268433</v>
+        <v>0.714297354221344</v>
       </c>
     </row>
     <row r="36">
@@ -8497,7 +8497,7 @@
         <v>0.132</v>
       </c>
       <c r="BO36" t="n">
-        <v>0.586679220199585</v>
+        <v>0.6608238816261292</v>
       </c>
     </row>
     <row r="37">
@@ -8718,7 +8718,7 @@
         <v>0</v>
       </c>
       <c r="BO37" t="n">
-        <v>0.7186930775642395</v>
+        <v>0.8220487236976624</v>
       </c>
     </row>
     <row r="38">
@@ -8939,7 +8939,7 @@
         <v>0</v>
       </c>
       <c r="BO38" t="n">
-        <v>0.726406455039978</v>
+        <v>0.7736412882804871</v>
       </c>
     </row>
     <row r="39">
@@ -9160,7 +9160,7 @@
         <v>0</v>
       </c>
       <c r="BO39" t="n">
-        <v>0.6043629050254822</v>
+        <v>0.4430015981197357</v>
       </c>
     </row>
     <row r="40">
@@ -9381,7 +9381,7 @@
         <v>0</v>
       </c>
       <c r="BO40" t="n">
-        <v>0.6481696963310242</v>
+        <v>0.6461691856384277</v>
       </c>
     </row>
     <row r="41">
@@ -9602,7 +9602,7 @@
         <v>0</v>
       </c>
       <c r="BO41" t="n">
-        <v>0.5931226015090942</v>
+        <v>0.4895467758178711</v>
       </c>
     </row>
     <row r="42">
@@ -9823,7 +9823,7 @@
         <v>0</v>
       </c>
       <c r="BO42" t="n">
-        <v>0.3309467434883118</v>
+        <v>0.4848021864891052</v>
       </c>
     </row>
     <row r="43">
@@ -10044,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="BO43" t="n">
-        <v>0.6775698065757751</v>
+        <v>0.6732003092765808</v>
       </c>
     </row>
     <row r="44">
@@ -10265,7 +10265,7 @@
         <v>0</v>
       </c>
       <c r="BO44" t="n">
-        <v>0.6773824095726013</v>
+        <v>0.6191999316215515</v>
       </c>
     </row>
     <row r="45">
@@ -10486,7 +10486,7 @@
         <v>0</v>
       </c>
       <c r="BO45" t="n">
-        <v>0.4398193359375</v>
+        <v>0.5700157284736633</v>
       </c>
     </row>
     <row r="46">
@@ -10707,7 +10707,7 @@
         <v>0</v>
       </c>
       <c r="BO46" t="n">
-        <v>0.4335010945796967</v>
+        <v>0.6737620830535889</v>
       </c>
     </row>
     <row r="47">
@@ -10928,7 +10928,7 @@
         <v>0</v>
       </c>
       <c r="BO47" t="n">
-        <v>0.8125020861625671</v>
+        <v>0.7631568312644958</v>
       </c>
     </row>
     <row r="48">
@@ -11149,7 +11149,7 @@
         <v>0</v>
       </c>
       <c r="BO48" t="n">
-        <v>0.7598451375961304</v>
+        <v>0.69390469789505</v>
       </c>
     </row>
     <row r="49">
@@ -11370,7 +11370,7 @@
         <v>0</v>
       </c>
       <c r="BO49" t="n">
-        <v>0.785118579864502</v>
+        <v>0.7028796076774597</v>
       </c>
     </row>
     <row r="50">
@@ -11591,7 +11591,7 @@
         <v>0</v>
       </c>
       <c r="BO50" t="n">
-        <v>0.7864914536476135</v>
+        <v>0.6760109066963196</v>
       </c>
     </row>
     <row r="51">
@@ -11812,7 +11812,7 @@
         <v>0</v>
       </c>
       <c r="BO51" t="n">
-        <v>0.7528362274169922</v>
+        <v>0.6505436301231384</v>
       </c>
     </row>
     <row r="52">
@@ -12033,7 +12033,7 @@
         <v>0</v>
       </c>
       <c r="BO52" t="n">
-        <v>0.3425798118114471</v>
+        <v>0.1117662787437439</v>
       </c>
     </row>
     <row r="53">
@@ -12254,7 +12254,7 @@
         <v>0</v>
       </c>
       <c r="BO53" t="n">
-        <v>0.08855804800987244</v>
+        <v>0.1265599876642227</v>
       </c>
     </row>
     <row r="54">
@@ -12475,7 +12475,7 @@
         <v>0</v>
       </c>
       <c r="BO54" t="n">
-        <v>0.1447912305593491</v>
+        <v>0.00934301596134901</v>
       </c>
     </row>
     <row r="55">
@@ -12696,7 +12696,7 @@
         <v>0</v>
       </c>
       <c r="BO55" t="n">
-        <v>0.6686598658561707</v>
+        <v>0.6037424206733704</v>
       </c>
     </row>
     <row r="56">
@@ -12917,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="BO56" t="n">
-        <v>0.769986093044281</v>
+        <v>0.7923555374145508</v>
       </c>
     </row>
     <row r="57">
@@ -13138,7 +13138,7 @@
         <v>0</v>
       </c>
       <c r="BO57" t="n">
-        <v>0.8110215067863464</v>
+        <v>0.6299933195114136</v>
       </c>
     </row>
     <row r="58">
@@ -13359,7 +13359,7 @@
         <v>0.219</v>
       </c>
       <c r="BO58" t="n">
-        <v>0.8314915299415588</v>
+        <v>0.8128296732902527</v>
       </c>
     </row>
     <row r="59">
@@ -13580,7 +13580,7 @@
         <v>0</v>
       </c>
       <c r="BO59" t="n">
-        <v>0.6956143379211426</v>
+        <v>0.7638512253761292</v>
       </c>
     </row>
     <row r="60">
@@ -13801,7 +13801,7 @@
         <v>0.094</v>
       </c>
       <c r="BO60" t="n">
-        <v>0.8052358627319336</v>
+        <v>0.8637326955795288</v>
       </c>
     </row>
     <row r="61">
@@ -14022,7 +14022,7 @@
         <v>0</v>
       </c>
       <c r="BO61" t="n">
-        <v>0.7711392045021057</v>
+        <v>0.7564572691917419</v>
       </c>
     </row>
     <row r="62">
@@ -14243,7 +14243,7 @@
         <v>0</v>
       </c>
       <c r="BO62" t="n">
-        <v>0.6761370301246643</v>
+        <v>0.7503859996795654</v>
       </c>
     </row>
     <row r="63">
@@ -14464,7 +14464,7 @@
         <v>0</v>
       </c>
       <c r="BO63" t="n">
-        <v>0.6755598187446594</v>
+        <v>0.6832898259162903</v>
       </c>
     </row>
     <row r="64">
@@ -14685,7 +14685,7 @@
         <v>0</v>
       </c>
       <c r="BO64" t="n">
-        <v>0.6819340586662292</v>
+        <v>0.6595971584320068</v>
       </c>
     </row>
     <row r="65">
@@ -14906,7 +14906,7 @@
         <v>0</v>
       </c>
       <c r="BO65" t="n">
-        <v>0.7015581727027893</v>
+        <v>0.6625831127166748</v>
       </c>
     </row>
     <row r="66">
@@ -15127,7 +15127,7 @@
         <v>0.073</v>
       </c>
       <c r="BO66" t="n">
-        <v>0.1775107830762863</v>
+        <v>0.08363591134548187</v>
       </c>
     </row>
     <row r="67">
@@ -15348,7 +15348,7 @@
         <v>0</v>
       </c>
       <c r="BO67" t="n">
-        <v>0.6487478613853455</v>
+        <v>0.6920419931411743</v>
       </c>
     </row>
     <row r="68">
@@ -15569,7 +15569,7 @@
         <v>0</v>
       </c>
       <c r="BO68" t="n">
-        <v>0.2301376610994339</v>
+        <v>0.04806749150156975</v>
       </c>
     </row>
     <row r="69">
@@ -15790,7 +15790,7 @@
         <v>0</v>
       </c>
       <c r="BO69" t="n">
-        <v>0.7196933031082153</v>
+        <v>0.6870089173316956</v>
       </c>
     </row>
     <row r="70">
@@ -16011,7 +16011,7 @@
         <v>0</v>
       </c>
       <c r="BO70" t="n">
-        <v>0.7267081737518311</v>
+        <v>0.6720928549766541</v>
       </c>
     </row>
     <row r="71">
@@ -16232,7 +16232,7 @@
         <v>0</v>
       </c>
       <c r="BO71" t="n">
-        <v>0.6877712607383728</v>
+        <v>0.7154821157455444</v>
       </c>
     </row>
     <row r="72">
@@ -16453,7 +16453,7 @@
         <v>0</v>
       </c>
       <c r="BO72" t="n">
-        <v>0.8070834875106812</v>
+        <v>0.719618558883667</v>
       </c>
     </row>
     <row r="73">
@@ -16674,7 +16674,7 @@
         <v>0</v>
       </c>
       <c r="BO73" t="n">
-        <v>0.7234486937522888</v>
+        <v>0.8204642534255981</v>
       </c>
     </row>
     <row r="74">
@@ -16895,7 +16895,7 @@
         <v>0</v>
       </c>
       <c r="BO74" t="n">
-        <v>0.659466028213501</v>
+        <v>0.8189181089401245</v>
       </c>
     </row>
     <row r="75">
@@ -17116,7 +17116,7 @@
         <v>0</v>
       </c>
       <c r="BO75" t="n">
-        <v>0.6659201383590698</v>
+        <v>0.7602909803390503</v>
       </c>
     </row>
     <row r="76">
@@ -17337,7 +17337,7 @@
         <v>0</v>
       </c>
       <c r="BO76" t="n">
-        <v>0.7721796631813049</v>
+        <v>0.7170021533966064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction of arguments parsing
</commit_message>
<xml_diff>
--- a/data/cohort-dataset-with-logreg-output.xlsx
+++ b/data/cohort-dataset-with-logreg-output.xlsx
@@ -983,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.8616690039634705</v>
+        <v>0.7651845216751099</v>
       </c>
     </row>
     <row r="3">
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.7642601728439331</v>
+        <v>0.6910622715950012</v>
       </c>
     </row>
     <row r="4">
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.8185211420059204</v>
+        <v>0.7168996930122375</v>
       </c>
     </row>
     <row r="5">
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.7934874892234802</v>
+        <v>0.8202211260795593</v>
       </c>
     </row>
     <row r="6">
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="BO6" t="n">
-        <v>0.7475650906562805</v>
+        <v>0.7839553952217102</v>
       </c>
     </row>
     <row r="7">
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="BO7" t="n">
-        <v>0.6309289336204529</v>
+        <v>0.7747849822044373</v>
       </c>
     </row>
     <row r="8">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.7830813527107239</v>
+        <v>0.8063458204269409</v>
       </c>
     </row>
     <row r="9">
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.8238789439201355</v>
+        <v>0.7721467614173889</v>
       </c>
     </row>
     <row r="10">
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="BO10" t="n">
-        <v>0.8128093481063843</v>
+        <v>0.6988649964332581</v>
       </c>
     </row>
     <row r="11">
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="BO11" t="n">
-        <v>0.6808183789253235</v>
+        <v>0.6677061915397644</v>
       </c>
     </row>
     <row r="12">
@@ -3193,7 +3193,7 @@
         <v>0</v>
       </c>
       <c r="BO12" t="n">
-        <v>0.7249404788017273</v>
+        <v>0.7753356695175171</v>
       </c>
     </row>
     <row r="13">
@@ -3414,7 +3414,7 @@
         <v>0</v>
       </c>
       <c r="BO13" t="n">
-        <v>0.7648003101348877</v>
+        <v>0.8061227798461914</v>
       </c>
     </row>
     <row r="14">
@@ -3635,7 +3635,7 @@
         <v>0</v>
       </c>
       <c r="BO14" t="n">
-        <v>0.8079110980033875</v>
+        <v>0.7610716819763184</v>
       </c>
     </row>
     <row r="15">
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="BO15" t="n">
-        <v>0.6319833993911743</v>
+        <v>0.724925696849823</v>
       </c>
     </row>
     <row r="16">
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
       <c r="BO16" t="n">
-        <v>0.808234691619873</v>
+        <v>0.6628627777099609</v>
       </c>
     </row>
     <row r="17">
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="BO17" t="n">
-        <v>0.8586356043815613</v>
+        <v>0.6985577344894409</v>
       </c>
     </row>
     <row r="18">
@@ -4519,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="BO18" t="n">
-        <v>0.6988104581832886</v>
+        <v>0.7677870392799377</v>
       </c>
     </row>
     <row r="19">
@@ -4740,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="BO19" t="n">
-        <v>0.4726418256759644</v>
+        <v>0.262258768081665</v>
       </c>
     </row>
     <row r="20">
@@ -4961,7 +4961,7 @@
         <v>0</v>
       </c>
       <c r="BO20" t="n">
-        <v>0.7849943041801453</v>
+        <v>0.7229638695716858</v>
       </c>
     </row>
     <row r="21">
@@ -5182,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="BO21" t="n">
-        <v>0.3410727977752686</v>
+        <v>0.5348628163337708</v>
       </c>
     </row>
     <row r="22">
@@ -5403,7 +5403,7 @@
         <v>0</v>
       </c>
       <c r="BO22" t="n">
-        <v>0.5046585202217102</v>
+        <v>0.526120126247406</v>
       </c>
     </row>
     <row r="23">
@@ -5624,7 +5624,7 @@
         <v>0.395</v>
       </c>
       <c r="BO23" t="n">
-        <v>0.7109943628311157</v>
+        <v>0.7717221975326538</v>
       </c>
     </row>
     <row r="24">
@@ -5845,7 +5845,7 @@
         <v>0</v>
       </c>
       <c r="BO24" t="n">
-        <v>0.7842209339141846</v>
+        <v>0.7844005823135376</v>
       </c>
     </row>
     <row r="25">
@@ -6066,7 +6066,7 @@
         <v>0</v>
       </c>
       <c r="BO25" t="n">
-        <v>0.5985342860221863</v>
+        <v>0.813689649105072</v>
       </c>
     </row>
     <row r="26">
@@ -6287,7 +6287,7 @@
         <v>0</v>
       </c>
       <c r="BO26" t="n">
-        <v>0.7847060561180115</v>
+        <v>0.7555526494979858</v>
       </c>
     </row>
     <row r="27">
@@ -6508,7 +6508,7 @@
         <v>0.11</v>
       </c>
       <c r="BO27" t="n">
-        <v>0.7347105741500854</v>
+        <v>0.6259112954139709</v>
       </c>
     </row>
     <row r="28">
@@ -6729,7 +6729,7 @@
         <v>0</v>
       </c>
       <c r="BO28" t="n">
-        <v>0.7248079776763916</v>
+        <v>0.6217015981674194</v>
       </c>
     </row>
     <row r="29">
@@ -6950,7 +6950,7 @@
         <v>0</v>
       </c>
       <c r="BO29" t="n">
-        <v>0.7834992408752441</v>
+        <v>0.8102371692657471</v>
       </c>
     </row>
     <row r="30">
@@ -7171,7 +7171,7 @@
         <v>0</v>
       </c>
       <c r="BO30" t="n">
-        <v>0.8199447393417358</v>
+        <v>0.8320518136024475</v>
       </c>
     </row>
     <row r="31">
@@ -7392,7 +7392,7 @@
         <v>0</v>
       </c>
       <c r="BO31" t="n">
-        <v>0.7464596629142761</v>
+        <v>0.6204785108566284</v>
       </c>
     </row>
     <row r="32">
@@ -7613,7 +7613,7 @@
         <v>0</v>
       </c>
       <c r="BO32" t="n">
-        <v>0.6721419095993042</v>
+        <v>0.6688506603240967</v>
       </c>
     </row>
     <row r="33">
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
       <c r="BO33" t="n">
-        <v>0.7016575336456299</v>
+        <v>0.8112037181854248</v>
       </c>
     </row>
     <row r="34">
@@ -8055,7 +8055,7 @@
         <v>0</v>
       </c>
       <c r="BO34" t="n">
-        <v>0.6511810421943665</v>
+        <v>0.4605306386947632</v>
       </c>
     </row>
     <row r="35">
@@ -8276,7 +8276,7 @@
         <v>0</v>
       </c>
       <c r="BO35" t="n">
-        <v>0.6883707046508789</v>
+        <v>0.7506204843521118</v>
       </c>
     </row>
     <row r="36">
@@ -8497,7 +8497,7 @@
         <v>0.132</v>
       </c>
       <c r="BO36" t="n">
-        <v>0.613903284072876</v>
+        <v>0.465054988861084</v>
       </c>
     </row>
     <row r="37">
@@ -8718,7 +8718,7 @@
         <v>0</v>
       </c>
       <c r="BO37" t="n">
-        <v>0.7432984113693237</v>
+        <v>0.7861714363098145</v>
       </c>
     </row>
     <row r="38">
@@ -8939,7 +8939,7 @@
         <v>0</v>
       </c>
       <c r="BO38" t="n">
-        <v>0.6608042120933533</v>
+        <v>0.6819479465484619</v>
       </c>
     </row>
     <row r="39">
@@ -9160,7 +9160,7 @@
         <v>0</v>
       </c>
       <c r="BO39" t="n">
-        <v>0.5536768436431885</v>
+        <v>0.6921868324279785</v>
       </c>
     </row>
     <row r="40">
@@ -9381,7 +9381,7 @@
         <v>0</v>
       </c>
       <c r="BO40" t="n">
-        <v>0.6508988738059998</v>
+        <v>0.6227372288703918</v>
       </c>
     </row>
     <row r="41">
@@ -9602,7 +9602,7 @@
         <v>0</v>
       </c>
       <c r="BO41" t="n">
-        <v>0.6809766888618469</v>
+        <v>0.4845716655254364</v>
       </c>
     </row>
     <row r="42">
@@ -9823,7 +9823,7 @@
         <v>0</v>
       </c>
       <c r="BO42" t="n">
-        <v>0.6687540411949158</v>
+        <v>0.4875307381153107</v>
       </c>
     </row>
     <row r="43">
@@ -10044,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="BO43" t="n">
-        <v>0.6269999146461487</v>
+        <v>0.6861420869827271</v>
       </c>
     </row>
     <row r="44">
@@ -10265,7 +10265,7 @@
         <v>0</v>
       </c>
       <c r="BO44" t="n">
-        <v>0.7277026772499084</v>
+        <v>0.7410923838615417</v>
       </c>
     </row>
     <row r="45">
@@ -10486,7 +10486,7 @@
         <v>0</v>
       </c>
       <c r="BO45" t="n">
-        <v>0.2194364070892334</v>
+        <v>0.5584484934806824</v>
       </c>
     </row>
     <row r="46">
@@ -10707,7 +10707,7 @@
         <v>0</v>
       </c>
       <c r="BO46" t="n">
-        <v>0.480913519859314</v>
+        <v>0.5410385727882385</v>
       </c>
     </row>
     <row r="47">
@@ -10928,7 +10928,7 @@
         <v>0</v>
       </c>
       <c r="BO47" t="n">
-        <v>0.8614972233772278</v>
+        <v>0.7851496338844299</v>
       </c>
     </row>
     <row r="48">
@@ -11149,7 +11149,7 @@
         <v>0</v>
       </c>
       <c r="BO48" t="n">
-        <v>0.717711865901947</v>
+        <v>0.7761016488075256</v>
       </c>
     </row>
     <row r="49">
@@ -11370,7 +11370,7 @@
         <v>0</v>
       </c>
       <c r="BO49" t="n">
-        <v>0.7972928285598755</v>
+        <v>0.7861425280570984</v>
       </c>
     </row>
     <row r="50">
@@ -11591,7 +11591,7 @@
         <v>0</v>
       </c>
       <c r="BO50" t="n">
-        <v>0.7888790965080261</v>
+        <v>0.7700994610786438</v>
       </c>
     </row>
     <row r="51">
@@ -11812,7 +11812,7 @@
         <v>0</v>
       </c>
       <c r="BO51" t="n">
-        <v>0.8026962876319885</v>
+        <v>0.8044094443321228</v>
       </c>
     </row>
     <row r="52">
@@ -12033,7 +12033,7 @@
         <v>0</v>
       </c>
       <c r="BO52" t="n">
-        <v>0.3527346253395081</v>
+        <v>0.5110746622085571</v>
       </c>
     </row>
     <row r="53">
@@ -12254,7 +12254,7 @@
         <v>0</v>
       </c>
       <c r="BO53" t="n">
-        <v>0.2097518593072891</v>
+        <v>0.06307589262723923</v>
       </c>
     </row>
     <row r="54">
@@ -12475,7 +12475,7 @@
         <v>0</v>
       </c>
       <c r="BO54" t="n">
-        <v>0.00564647139981389</v>
+        <v>0.01375659089535475</v>
       </c>
     </row>
     <row r="55">
@@ -12696,7 +12696,7 @@
         <v>0</v>
       </c>
       <c r="BO55" t="n">
-        <v>0.7036200165748596</v>
+        <v>0.7130152583122253</v>
       </c>
     </row>
     <row r="56">
@@ -12917,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="BO56" t="n">
-        <v>0.8753008842468262</v>
+        <v>0.8709108233451843</v>
       </c>
     </row>
     <row r="57">
@@ -13138,7 +13138,7 @@
         <v>0</v>
       </c>
       <c r="BO57" t="n">
-        <v>0.7501981854438782</v>
+        <v>0.8509075045585632</v>
       </c>
     </row>
     <row r="58">
@@ -13359,7 +13359,7 @@
         <v>0.219</v>
       </c>
       <c r="BO58" t="n">
-        <v>0.6285371780395508</v>
+        <v>0.993416428565979</v>
       </c>
     </row>
     <row r="59">
@@ -13580,7 +13580,7 @@
         <v>0</v>
       </c>
       <c r="BO59" t="n">
-        <v>0.8092096447944641</v>
+        <v>0.8836907148361206</v>
       </c>
     </row>
     <row r="60">
@@ -13801,7 +13801,7 @@
         <v>0.094</v>
       </c>
       <c r="BO60" t="n">
-        <v>0.8402552008628845</v>
+        <v>0.7212737798690796</v>
       </c>
     </row>
     <row r="61">
@@ -14022,7 +14022,7 @@
         <v>0</v>
       </c>
       <c r="BO61" t="n">
-        <v>0.8609434962272644</v>
+        <v>0.8123336434364319</v>
       </c>
     </row>
     <row r="62">
@@ -14243,7 +14243,7 @@
         <v>0</v>
       </c>
       <c r="BO62" t="n">
-        <v>0.8365370631217957</v>
+        <v>0.795131504535675</v>
       </c>
     </row>
     <row r="63">
@@ -14464,7 +14464,7 @@
         <v>0</v>
       </c>
       <c r="BO63" t="n">
-        <v>0.6875803470611572</v>
+        <v>0.6210874915122986</v>
       </c>
     </row>
     <row r="64">
@@ -14685,7 +14685,7 @@
         <v>0</v>
       </c>
       <c r="BO64" t="n">
-        <v>0.695228636264801</v>
+        <v>0.7399969696998596</v>
       </c>
     </row>
     <row r="65">
@@ -14906,7 +14906,7 @@
         <v>0</v>
       </c>
       <c r="BO65" t="n">
-        <v>0.724416971206665</v>
+        <v>0.7289398312568665</v>
       </c>
     </row>
     <row r="66">
@@ -15127,7 +15127,7 @@
         <v>0.073</v>
       </c>
       <c r="BO66" t="n">
-        <v>0.1853055208921432</v>
+        <v>0.01506303902715445</v>
       </c>
     </row>
     <row r="67">
@@ -15348,7 +15348,7 @@
         <v>0</v>
       </c>
       <c r="BO67" t="n">
-        <v>0.6737421751022339</v>
+        <v>0.6572929620742798</v>
       </c>
     </row>
     <row r="68">
@@ -15569,7 +15569,7 @@
         <v>0</v>
       </c>
       <c r="BO68" t="n">
-        <v>0.07274846732616425</v>
+        <v>0.06046081334352493</v>
       </c>
     </row>
     <row r="69">
@@ -15790,7 +15790,7 @@
         <v>0</v>
       </c>
       <c r="BO69" t="n">
-        <v>0.6591382026672363</v>
+        <v>0.722989559173584</v>
       </c>
     </row>
     <row r="70">
@@ -16011,7 +16011,7 @@
         <v>0</v>
       </c>
       <c r="BO70" t="n">
-        <v>0.6616680026054382</v>
+        <v>0.7818295955657959</v>
       </c>
     </row>
     <row r="71">
@@ -16232,7 +16232,7 @@
         <v>0</v>
       </c>
       <c r="BO71" t="n">
-        <v>0.5536182522773743</v>
+        <v>0.3541120290756226</v>
       </c>
     </row>
     <row r="72">
@@ -16453,7 +16453,7 @@
         <v>0</v>
       </c>
       <c r="BO72" t="n">
-        <v>0.7583860158920288</v>
+        <v>0.7111461758613586</v>
       </c>
     </row>
     <row r="73">
@@ -16674,7 +16674,7 @@
         <v>0</v>
       </c>
       <c r="BO73" t="n">
-        <v>0.7928439974784851</v>
+        <v>0.758787214756012</v>
       </c>
     </row>
     <row r="74">
@@ -16895,7 +16895,7 @@
         <v>0</v>
       </c>
       <c r="BO74" t="n">
-        <v>0.6749022006988525</v>
+        <v>0.7623749971389771</v>
       </c>
     </row>
     <row r="75">
@@ -17116,7 +17116,7 @@
         <v>0</v>
       </c>
       <c r="BO75" t="n">
-        <v>0.8374364972114563</v>
+        <v>0.6713321208953857</v>
       </c>
     </row>
     <row r="76">
@@ -17337,7 +17337,7 @@
         <v>0</v>
       </c>
       <c r="BO76" t="n">
-        <v>0.8474271297454834</v>
+        <v>0.7403024435043335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
encapsulate in functions for main scripts
</commit_message>
<xml_diff>
--- a/data/cohort-dataset-with-logreg-output.xlsx
+++ b/data/cohort-dataset-with-logreg-output.xlsx
@@ -983,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.7651845216751099</v>
+        <v>0.707798182964325</v>
       </c>
     </row>
     <row r="3">
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.6910622715950012</v>
+        <v>0.7345734238624573</v>
       </c>
     </row>
     <row r="4">
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.7168996930122375</v>
+        <v>0.8727198243141174</v>
       </c>
     </row>
     <row r="5">
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.8202211260795593</v>
+        <v>0.8167624473571777</v>
       </c>
     </row>
     <row r="6">
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="BO6" t="n">
-        <v>0.7839553952217102</v>
+        <v>0.7034626007080078</v>
       </c>
     </row>
     <row r="7">
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="BO7" t="n">
-        <v>0.7747849822044373</v>
+        <v>0.6226551532745361</v>
       </c>
     </row>
     <row r="8">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.8063458204269409</v>
+        <v>0.7518402934074402</v>
       </c>
     </row>
     <row r="9">
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.7721467614173889</v>
+        <v>0.7594751715660095</v>
       </c>
     </row>
     <row r="10">
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="BO10" t="n">
-        <v>0.6988649964332581</v>
+        <v>0.7373155355453491</v>
       </c>
     </row>
     <row r="11">
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="BO11" t="n">
-        <v>0.6677061915397644</v>
+        <v>0.7546300292015076</v>
       </c>
     </row>
     <row r="12">
@@ -3193,7 +3193,7 @@
         <v>0</v>
       </c>
       <c r="BO12" t="n">
-        <v>0.7753356695175171</v>
+        <v>0.6847510933876038</v>
       </c>
     </row>
     <row r="13">
@@ -3414,7 +3414,7 @@
         <v>0</v>
       </c>
       <c r="BO13" t="n">
-        <v>0.8061227798461914</v>
+        <v>0.7531487345695496</v>
       </c>
     </row>
     <row r="14">
@@ -3635,7 +3635,7 @@
         <v>0</v>
       </c>
       <c r="BO14" t="n">
-        <v>0.7610716819763184</v>
+        <v>0.650474488735199</v>
       </c>
     </row>
     <row r="15">
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="BO15" t="n">
-        <v>0.724925696849823</v>
+        <v>0.6719115972518921</v>
       </c>
     </row>
     <row r="16">
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
       <c r="BO16" t="n">
-        <v>0.6628627777099609</v>
+        <v>0.7176676392555237</v>
       </c>
     </row>
     <row r="17">
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="BO17" t="n">
-        <v>0.6985577344894409</v>
+        <v>0.7194453477859497</v>
       </c>
     </row>
     <row r="18">
@@ -4519,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="BO18" t="n">
-        <v>0.7677870392799377</v>
+        <v>0.7973012924194336</v>
       </c>
     </row>
     <row r="19">
@@ -4740,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="BO19" t="n">
-        <v>0.262258768081665</v>
+        <v>0.4688084423542023</v>
       </c>
     </row>
     <row r="20">
@@ -4961,7 +4961,7 @@
         <v>0</v>
       </c>
       <c r="BO20" t="n">
-        <v>0.7229638695716858</v>
+        <v>0.7541728615760803</v>
       </c>
     </row>
     <row r="21">
@@ -5182,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="BO21" t="n">
-        <v>0.5348628163337708</v>
+        <v>0.4263558387756348</v>
       </c>
     </row>
     <row r="22">
@@ -5403,7 +5403,7 @@
         <v>0</v>
       </c>
       <c r="BO22" t="n">
-        <v>0.526120126247406</v>
+        <v>0.6458883285522461</v>
       </c>
     </row>
     <row r="23">
@@ -5624,7 +5624,7 @@
         <v>0.395</v>
       </c>
       <c r="BO23" t="n">
-        <v>0.7717221975326538</v>
+        <v>0.8448514938354492</v>
       </c>
     </row>
     <row r="24">
@@ -5845,7 +5845,7 @@
         <v>0</v>
       </c>
       <c r="BO24" t="n">
-        <v>0.7844005823135376</v>
+        <v>0.8312001824378967</v>
       </c>
     </row>
     <row r="25">
@@ -6066,7 +6066,7 @@
         <v>0</v>
       </c>
       <c r="BO25" t="n">
-        <v>0.813689649105072</v>
+        <v>0.7239437103271484</v>
       </c>
     </row>
     <row r="26">
@@ -6287,7 +6287,7 @@
         <v>0</v>
       </c>
       <c r="BO26" t="n">
-        <v>0.7555526494979858</v>
+        <v>0.7627598643302917</v>
       </c>
     </row>
     <row r="27">
@@ -6508,7 +6508,7 @@
         <v>0.11</v>
       </c>
       <c r="BO27" t="n">
-        <v>0.6259112954139709</v>
+        <v>0.834860622882843</v>
       </c>
     </row>
     <row r="28">
@@ -6729,7 +6729,7 @@
         <v>0</v>
       </c>
       <c r="BO28" t="n">
-        <v>0.6217015981674194</v>
+        <v>0.7576714158058167</v>
       </c>
     </row>
     <row r="29">
@@ -6950,7 +6950,7 @@
         <v>0</v>
       </c>
       <c r="BO29" t="n">
-        <v>0.8102371692657471</v>
+        <v>0.7069045901298523</v>
       </c>
     </row>
     <row r="30">
@@ -7171,7 +7171,7 @@
         <v>0</v>
       </c>
       <c r="BO30" t="n">
-        <v>0.8320518136024475</v>
+        <v>0.7657533884048462</v>
       </c>
     </row>
     <row r="31">
@@ -7392,7 +7392,7 @@
         <v>0</v>
       </c>
       <c r="BO31" t="n">
-        <v>0.6204785108566284</v>
+        <v>0.7477073073387146</v>
       </c>
     </row>
     <row r="32">
@@ -7613,7 +7613,7 @@
         <v>0</v>
       </c>
       <c r="BO32" t="n">
-        <v>0.6688506603240967</v>
+        <v>0.5232943892478943</v>
       </c>
     </row>
     <row r="33">
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
       <c r="BO33" t="n">
-        <v>0.8112037181854248</v>
+        <v>0.6623345613479614</v>
       </c>
     </row>
     <row r="34">
@@ -8055,7 +8055,7 @@
         <v>0</v>
       </c>
       <c r="BO34" t="n">
-        <v>0.4605306386947632</v>
+        <v>0.766302227973938</v>
       </c>
     </row>
     <row r="35">
@@ -8276,7 +8276,7 @@
         <v>0</v>
       </c>
       <c r="BO35" t="n">
-        <v>0.7506204843521118</v>
+        <v>0.7689911723136902</v>
       </c>
     </row>
     <row r="36">
@@ -8497,7 +8497,7 @@
         <v>0.132</v>
       </c>
       <c r="BO36" t="n">
-        <v>0.465054988861084</v>
+        <v>0.5299518704414368</v>
       </c>
     </row>
     <row r="37">
@@ -8718,7 +8718,7 @@
         <v>0</v>
       </c>
       <c r="BO37" t="n">
-        <v>0.7861714363098145</v>
+        <v>0.7659668326377869</v>
       </c>
     </row>
     <row r="38">
@@ -8939,7 +8939,7 @@
         <v>0</v>
       </c>
       <c r="BO38" t="n">
-        <v>0.6819479465484619</v>
+        <v>0.7795442342758179</v>
       </c>
     </row>
     <row r="39">
@@ -9160,7 +9160,7 @@
         <v>0</v>
       </c>
       <c r="BO39" t="n">
-        <v>0.6921868324279785</v>
+        <v>0.466173529624939</v>
       </c>
     </row>
     <row r="40">
@@ -9381,7 +9381,7 @@
         <v>0</v>
       </c>
       <c r="BO40" t="n">
-        <v>0.6227372288703918</v>
+        <v>0.7568145394325256</v>
       </c>
     </row>
     <row r="41">
@@ -9602,7 +9602,7 @@
         <v>0</v>
       </c>
       <c r="BO41" t="n">
-        <v>0.4845716655254364</v>
+        <v>0.5414235591888428</v>
       </c>
     </row>
     <row r="42">
@@ -9823,7 +9823,7 @@
         <v>0</v>
       </c>
       <c r="BO42" t="n">
-        <v>0.4875307381153107</v>
+        <v>0.6749743819236755</v>
       </c>
     </row>
     <row r="43">
@@ -10044,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="BO43" t="n">
-        <v>0.6861420869827271</v>
+        <v>0.6900009512901306</v>
       </c>
     </row>
     <row r="44">
@@ -10265,7 +10265,7 @@
         <v>0</v>
       </c>
       <c r="BO44" t="n">
-        <v>0.7410923838615417</v>
+        <v>0.7264436483383179</v>
       </c>
     </row>
     <row r="45">
@@ -10486,7 +10486,7 @@
         <v>0</v>
       </c>
       <c r="BO45" t="n">
-        <v>0.5584484934806824</v>
+        <v>0.4763390123844147</v>
       </c>
     </row>
     <row r="46">
@@ -10707,7 +10707,7 @@
         <v>0</v>
       </c>
       <c r="BO46" t="n">
-        <v>0.5410385727882385</v>
+        <v>0.4493989646434784</v>
       </c>
     </row>
     <row r="47">
@@ -10928,7 +10928,7 @@
         <v>0</v>
       </c>
       <c r="BO47" t="n">
-        <v>0.7851496338844299</v>
+        <v>0.8399074673652649</v>
       </c>
     </row>
     <row r="48">
@@ -11149,7 +11149,7 @@
         <v>0</v>
       </c>
       <c r="BO48" t="n">
-        <v>0.7761016488075256</v>
+        <v>0.8476596474647522</v>
       </c>
     </row>
     <row r="49">
@@ -11370,7 +11370,7 @@
         <v>0</v>
       </c>
       <c r="BO49" t="n">
-        <v>0.7861425280570984</v>
+        <v>0.801840603351593</v>
       </c>
     </row>
     <row r="50">
@@ -11591,7 +11591,7 @@
         <v>0</v>
       </c>
       <c r="BO50" t="n">
-        <v>0.7700994610786438</v>
+        <v>0.8449442386627197</v>
       </c>
     </row>
     <row r="51">
@@ -11812,7 +11812,7 @@
         <v>0</v>
       </c>
       <c r="BO51" t="n">
-        <v>0.8044094443321228</v>
+        <v>0.7922573685646057</v>
       </c>
     </row>
     <row r="52">
@@ -12033,7 +12033,7 @@
         <v>0</v>
       </c>
       <c r="BO52" t="n">
-        <v>0.5110746622085571</v>
+        <v>0.5533796548843384</v>
       </c>
     </row>
     <row r="53">
@@ -12254,7 +12254,7 @@
         <v>0</v>
       </c>
       <c r="BO53" t="n">
-        <v>0.06307589262723923</v>
+        <v>0.1368321627378464</v>
       </c>
     </row>
     <row r="54">
@@ -12475,7 +12475,7 @@
         <v>0</v>
       </c>
       <c r="BO54" t="n">
-        <v>0.01375659089535475</v>
+        <v>0.07053074240684509</v>
       </c>
     </row>
     <row r="55">
@@ -12696,7 +12696,7 @@
         <v>0</v>
       </c>
       <c r="BO55" t="n">
-        <v>0.7130152583122253</v>
+        <v>0.7324074506759644</v>
       </c>
     </row>
     <row r="56">
@@ -12917,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="BO56" t="n">
-        <v>0.8709108233451843</v>
+        <v>0.7779104113578796</v>
       </c>
     </row>
     <row r="57">
@@ -13138,7 +13138,7 @@
         <v>0</v>
       </c>
       <c r="BO57" t="n">
-        <v>0.8509075045585632</v>
+        <v>0.8202462792396545</v>
       </c>
     </row>
     <row r="58">
@@ -13359,7 +13359,7 @@
         <v>0.219</v>
       </c>
       <c r="BO58" t="n">
-        <v>0.993416428565979</v>
+        <v>0.9326225519180298</v>
       </c>
     </row>
     <row r="59">
@@ -13580,7 +13580,7 @@
         <v>0</v>
       </c>
       <c r="BO59" t="n">
-        <v>0.8836907148361206</v>
+        <v>0.7098234295845032</v>
       </c>
     </row>
     <row r="60">
@@ -13801,7 +13801,7 @@
         <v>0.094</v>
       </c>
       <c r="BO60" t="n">
-        <v>0.7212737798690796</v>
+        <v>0.8557806015014648</v>
       </c>
     </row>
     <row r="61">
@@ -14022,7 +14022,7 @@
         <v>0</v>
       </c>
       <c r="BO61" t="n">
-        <v>0.8123336434364319</v>
+        <v>0.8278502821922302</v>
       </c>
     </row>
     <row r="62">
@@ -14243,7 +14243,7 @@
         <v>0</v>
       </c>
       <c r="BO62" t="n">
-        <v>0.795131504535675</v>
+        <v>0.8157700896263123</v>
       </c>
     </row>
     <row r="63">
@@ -14464,7 +14464,7 @@
         <v>0</v>
       </c>
       <c r="BO63" t="n">
-        <v>0.6210874915122986</v>
+        <v>0.6926621794700623</v>
       </c>
     </row>
     <row r="64">
@@ -14685,7 +14685,7 @@
         <v>0</v>
       </c>
       <c r="BO64" t="n">
-        <v>0.7399969696998596</v>
+        <v>0.7022183537483215</v>
       </c>
     </row>
     <row r="65">
@@ -14906,7 +14906,7 @@
         <v>0</v>
       </c>
       <c r="BO65" t="n">
-        <v>0.7289398312568665</v>
+        <v>0.7145379185676575</v>
       </c>
     </row>
     <row r="66">
@@ -15127,7 +15127,7 @@
         <v>0.073</v>
       </c>
       <c r="BO66" t="n">
-        <v>0.01506303902715445</v>
+        <v>0.1714053452014923</v>
       </c>
     </row>
     <row r="67">
@@ -15348,7 +15348,7 @@
         <v>0</v>
       </c>
       <c r="BO67" t="n">
-        <v>0.6572929620742798</v>
+        <v>0.6154088377952576</v>
       </c>
     </row>
     <row r="68">
@@ -15569,7 +15569,7 @@
         <v>0</v>
       </c>
       <c r="BO68" t="n">
-        <v>0.06046081334352493</v>
+        <v>0.3205895125865936</v>
       </c>
     </row>
     <row r="69">
@@ -15790,7 +15790,7 @@
         <v>0</v>
       </c>
       <c r="BO69" t="n">
-        <v>0.722989559173584</v>
+        <v>0.8269971013069153</v>
       </c>
     </row>
     <row r="70">
@@ -16011,7 +16011,7 @@
         <v>0</v>
       </c>
       <c r="BO70" t="n">
-        <v>0.7818295955657959</v>
+        <v>0.8011592626571655</v>
       </c>
     </row>
     <row r="71">
@@ -16232,7 +16232,7 @@
         <v>0</v>
       </c>
       <c r="BO71" t="n">
-        <v>0.3541120290756226</v>
+        <v>0.6300471425056458</v>
       </c>
     </row>
     <row r="72">
@@ -16453,7 +16453,7 @@
         <v>0</v>
       </c>
       <c r="BO72" t="n">
-        <v>0.7111461758613586</v>
+        <v>0.6852648854255676</v>
       </c>
     </row>
     <row r="73">
@@ -16674,7 +16674,7 @@
         <v>0</v>
       </c>
       <c r="BO73" t="n">
-        <v>0.758787214756012</v>
+        <v>0.8271722197532654</v>
       </c>
     </row>
     <row r="74">
@@ -16895,7 +16895,7 @@
         <v>0</v>
       </c>
       <c r="BO74" t="n">
-        <v>0.7623749971389771</v>
+        <v>0.7276062965393066</v>
       </c>
     </row>
     <row r="75">
@@ -17116,7 +17116,7 @@
         <v>0</v>
       </c>
       <c r="BO75" t="n">
-        <v>0.6713321208953857</v>
+        <v>0.8522377014160156</v>
       </c>
     </row>
     <row r="76">
@@ -17337,7 +17337,7 @@
         <v>0</v>
       </c>
       <c r="BO76" t="n">
-        <v>0.7403024435043335</v>
+        <v>0.8691616058349609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
classification threshold in parameter
</commit_message>
<xml_diff>
--- a/data/cohort-dataset-with-logreg-output.xlsx
+++ b/data/cohort-dataset-with-logreg-output.xlsx
@@ -983,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="BO2" t="n">
-        <v>0.8139268755912781</v>
+        <v>0.7000501751899719</v>
       </c>
     </row>
     <row r="3">
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="BO3" t="n">
-        <v>0.6964861750602722</v>
+        <v>0.7252546548843384</v>
       </c>
     </row>
     <row r="4">
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.7521433234214783</v>
+        <v>0.8770965337753296</v>
       </c>
     </row>
     <row r="5">
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.7041338682174683</v>
+        <v>0.726647675037384</v>
       </c>
     </row>
     <row r="6">
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="BO6" t="n">
-        <v>0.7659457921981812</v>
+        <v>0.752899169921875</v>
       </c>
     </row>
     <row r="7">
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="BO7" t="n">
-        <v>0.7237898707389832</v>
+        <v>0.7230728268623352</v>
       </c>
     </row>
     <row r="8">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.7575628161430359</v>
+        <v>0.7775186896324158</v>
       </c>
     </row>
     <row r="9">
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.8326842784881592</v>
+        <v>0.7579985857009888</v>
       </c>
     </row>
     <row r="10">
@@ -2751,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="BO10" t="n">
-        <v>0.7770835757255554</v>
+        <v>0.729798436164856</v>
       </c>
     </row>
     <row r="11">
@@ -2972,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="BO11" t="n">
-        <v>0.7281512022018433</v>
+        <v>0.7400994896888733</v>
       </c>
     </row>
     <row r="12">
@@ -3193,7 +3193,7 @@
         <v>0</v>
       </c>
       <c r="BO12" t="n">
-        <v>0.7310398817062378</v>
+        <v>0.7421934008598328</v>
       </c>
     </row>
     <row r="13">
@@ -3414,7 +3414,7 @@
         <v>0</v>
       </c>
       <c r="BO13" t="n">
-        <v>0.7169790267944336</v>
+        <v>0.7053585052490234</v>
       </c>
     </row>
     <row r="14">
@@ -3635,7 +3635,7 @@
         <v>0</v>
       </c>
       <c r="BO14" t="n">
-        <v>0.6863900423049927</v>
+        <v>0.7672739624977112</v>
       </c>
     </row>
     <row r="15">
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="BO15" t="n">
-        <v>0.5470817089080811</v>
+        <v>0.6614869236946106</v>
       </c>
     </row>
     <row r="16">
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
       <c r="BO16" t="n">
-        <v>0.7225398421287537</v>
+        <v>0.7542528510093689</v>
       </c>
     </row>
     <row r="17">
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="BO17" t="n">
-        <v>0.7759443521499634</v>
+        <v>0.7394630908966064</v>
       </c>
     </row>
     <row r="18">
@@ -4519,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="BO18" t="n">
-        <v>0.7508914470672607</v>
+        <v>0.7813862562179565</v>
       </c>
     </row>
     <row r="19">
@@ -4740,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="BO19" t="n">
-        <v>0.6337060928344727</v>
+        <v>0.345298707485199</v>
       </c>
     </row>
     <row r="20">
@@ -4961,7 +4961,7 @@
         <v>0</v>
       </c>
       <c r="BO20" t="n">
-        <v>0.778674840927124</v>
+        <v>0.7774925231933594</v>
       </c>
     </row>
     <row r="21">
@@ -5182,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="BO21" t="n">
-        <v>0.3754101097583771</v>
+        <v>0.4294066727161407</v>
       </c>
     </row>
     <row r="22">
@@ -5403,7 +5403,7 @@
         <v>0</v>
       </c>
       <c r="BO22" t="n">
-        <v>0.6097265481948853</v>
+        <v>0.4785134196281433</v>
       </c>
     </row>
     <row r="23">
@@ -5624,7 +5624,7 @@
         <v>0.395</v>
       </c>
       <c r="BO23" t="n">
-        <v>0.7117049098014832</v>
+        <v>0.7571130990982056</v>
       </c>
     </row>
     <row r="24">
@@ -5845,7 +5845,7 @@
         <v>0</v>
       </c>
       <c r="BO24" t="n">
-        <v>0.790002167224884</v>
+        <v>0.6992326378822327</v>
       </c>
     </row>
     <row r="25">
@@ -6066,7 +6066,7 @@
         <v>0</v>
       </c>
       <c r="BO25" t="n">
-        <v>0.7576935887336731</v>
+        <v>0.6605466604232788</v>
       </c>
     </row>
     <row r="26">
@@ -6287,7 +6287,7 @@
         <v>0</v>
       </c>
       <c r="BO26" t="n">
-        <v>0.7795416712760925</v>
+        <v>0.71180659532547</v>
       </c>
     </row>
     <row r="27">
@@ -6508,7 +6508,7 @@
         <v>0.11</v>
       </c>
       <c r="BO27" t="n">
-        <v>0.6405622959136963</v>
+        <v>0.6626912355422974</v>
       </c>
     </row>
     <row r="28">
@@ -6729,7 +6729,7 @@
         <v>0</v>
       </c>
       <c r="BO28" t="n">
-        <v>0.6373890042304993</v>
+        <v>0.6601747274398804</v>
       </c>
     </row>
     <row r="29">
@@ -6950,7 +6950,7 @@
         <v>0</v>
       </c>
       <c r="BO29" t="n">
-        <v>0.6548123359680176</v>
+        <v>0.6637101173400879</v>
       </c>
     </row>
     <row r="30">
@@ -7171,7 +7171,7 @@
         <v>0</v>
       </c>
       <c r="BO30" t="n">
-        <v>0.7234230637550354</v>
+        <v>0.7701870799064636</v>
       </c>
     </row>
     <row r="31">
@@ -7392,7 +7392,7 @@
         <v>0</v>
       </c>
       <c r="BO31" t="n">
-        <v>0.6595823168754578</v>
+        <v>0.7080376744270325</v>
       </c>
     </row>
     <row r="32">
@@ -7613,7 +7613,7 @@
         <v>0</v>
       </c>
       <c r="BO32" t="n">
-        <v>0.5564994215965271</v>
+        <v>0.5439549088478088</v>
       </c>
     </row>
     <row r="33">
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
       <c r="BO33" t="n">
-        <v>0.7224302887916565</v>
+        <v>0.6939806938171387</v>
       </c>
     </row>
     <row r="34">
@@ -8055,7 +8055,7 @@
         <v>0</v>
       </c>
       <c r="BO34" t="n">
-        <v>0.6448922753334045</v>
+        <v>0.5539235472679138</v>
       </c>
     </row>
     <row r="35">
@@ -8276,7 +8276,7 @@
         <v>0</v>
       </c>
       <c r="BO35" t="n">
-        <v>0.7193447351455688</v>
+        <v>0.7407917380332947</v>
       </c>
     </row>
     <row r="36">
@@ -8497,7 +8497,7 @@
         <v>0.132</v>
       </c>
       <c r="BO36" t="n">
-        <v>0.5413621068000793</v>
+        <v>0.5644567012786865</v>
       </c>
     </row>
     <row r="37">
@@ -8718,7 +8718,7 @@
         <v>0</v>
       </c>
       <c r="BO37" t="n">
-        <v>0.8032723069190979</v>
+        <v>0.8088090419769287</v>
       </c>
     </row>
     <row r="38">
@@ -8939,7 +8939,7 @@
         <v>0</v>
       </c>
       <c r="BO38" t="n">
-        <v>0.7108537554740906</v>
+        <v>0.6603132486343384</v>
       </c>
     </row>
     <row r="39">
@@ -9160,7 +9160,7 @@
         <v>0</v>
       </c>
       <c r="BO39" t="n">
-        <v>0.4838632941246033</v>
+        <v>0.6831006407737732</v>
       </c>
     </row>
     <row r="40">
@@ -9381,7 +9381,7 @@
         <v>0</v>
       </c>
       <c r="BO40" t="n">
-        <v>0.697007417678833</v>
+        <v>0.6939290761947632</v>
       </c>
     </row>
     <row r="41">
@@ -9602,7 +9602,7 @@
         <v>0</v>
       </c>
       <c r="BO41" t="n">
-        <v>0.691240668296814</v>
+        <v>0.5631906390190125</v>
       </c>
     </row>
     <row r="42">
@@ -9823,7 +9823,7 @@
         <v>0</v>
       </c>
       <c r="BO42" t="n">
-        <v>0.4123856127262115</v>
+        <v>0.49684077501297</v>
       </c>
     </row>
     <row r="43">
@@ -10044,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="BO43" t="n">
-        <v>0.6324948072433472</v>
+        <v>0.5076735019683838</v>
       </c>
     </row>
     <row r="44">
@@ -10265,7 +10265,7 @@
         <v>0</v>
       </c>
       <c r="BO44" t="n">
-        <v>0.5550192594528198</v>
+        <v>0.7261407375335693</v>
       </c>
     </row>
     <row r="45">
@@ -10486,7 +10486,7 @@
         <v>0</v>
       </c>
       <c r="BO45" t="n">
-        <v>0.4910290241241455</v>
+        <v>0.5679957866668701</v>
       </c>
     </row>
     <row r="46">
@@ -10707,7 +10707,7 @@
         <v>0</v>
       </c>
       <c r="BO46" t="n">
-        <v>0.2608720064163208</v>
+        <v>0.457265168428421</v>
       </c>
     </row>
     <row r="47">
@@ -10928,7 +10928,7 @@
         <v>0</v>
       </c>
       <c r="BO47" t="n">
-        <v>0.7454967498779297</v>
+        <v>0.7280606031417847</v>
       </c>
     </row>
     <row r="48">
@@ -11149,7 +11149,7 @@
         <v>0</v>
       </c>
       <c r="BO48" t="n">
-        <v>0.7300103902816772</v>
+        <v>0.7098612785339355</v>
       </c>
     </row>
     <row r="49">
@@ -11370,7 +11370,7 @@
         <v>0</v>
       </c>
       <c r="BO49" t="n">
-        <v>0.6161171793937683</v>
+        <v>0.7323701977729797</v>
       </c>
     </row>
     <row r="50">
@@ -11591,7 +11591,7 @@
         <v>0</v>
       </c>
       <c r="BO50" t="n">
-        <v>0.7688886523246765</v>
+        <v>0.7484275102615356</v>
       </c>
     </row>
     <row r="51">
@@ -11812,7 +11812,7 @@
         <v>0</v>
       </c>
       <c r="BO51" t="n">
-        <v>0.7004209756851196</v>
+        <v>0.6802716851234436</v>
       </c>
     </row>
     <row r="52">
@@ -12033,7 +12033,7 @@
         <v>0</v>
       </c>
       <c r="BO52" t="n">
-        <v>0.1795154511928558</v>
+        <v>0.322256863117218</v>
       </c>
     </row>
     <row r="53">
@@ -12254,7 +12254,7 @@
         <v>0</v>
       </c>
       <c r="BO53" t="n">
-        <v>0.1804946511983871</v>
+        <v>0.2477652579545975</v>
       </c>
     </row>
     <row r="54">
@@ -12475,7 +12475,7 @@
         <v>0</v>
       </c>
       <c r="BO54" t="n">
-        <v>0.004290489014238119</v>
+        <v>0.005304196383804083</v>
       </c>
     </row>
     <row r="55">
@@ -12696,7 +12696,7 @@
         <v>0</v>
       </c>
       <c r="BO55" t="n">
-        <v>0.7002317309379578</v>
+        <v>0.7294290661811829</v>
       </c>
     </row>
     <row r="56">
@@ -12917,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="BO56" t="n">
-        <v>0.6815613508224487</v>
+        <v>0.8103954195976257</v>
       </c>
     </row>
     <row r="57">
@@ -13138,7 +13138,7 @@
         <v>0</v>
       </c>
       <c r="BO57" t="n">
-        <v>0.7090147733688354</v>
+        <v>0.7873294353485107</v>
       </c>
     </row>
     <row r="58">
@@ -13359,7 +13359,7 @@
         <v>0.219</v>
       </c>
       <c r="BO58" t="n">
-        <v>0.9372679591178894</v>
+        <v>0.02227035723626614</v>
       </c>
     </row>
     <row r="59">
@@ -13580,7 +13580,7 @@
         <v>0</v>
       </c>
       <c r="BO59" t="n">
-        <v>0.7824841737747192</v>
+        <v>0.7275230288505554</v>
       </c>
     </row>
     <row r="60">
@@ -13801,7 +13801,7 @@
         <v>0.094</v>
       </c>
       <c r="BO60" t="n">
-        <v>0.8074166774749756</v>
+        <v>0.7685961723327637</v>
       </c>
     </row>
     <row r="61">
@@ -14022,7 +14022,7 @@
         <v>0</v>
       </c>
       <c r="BO61" t="n">
-        <v>0.79543137550354</v>
+        <v>0.7116091251373291</v>
       </c>
     </row>
     <row r="62">
@@ -14243,7 +14243,7 @@
         <v>0</v>
       </c>
       <c r="BO62" t="n">
-        <v>0.7869144678115845</v>
+        <v>0.7875267267227173</v>
       </c>
     </row>
     <row r="63">
@@ -14464,7 +14464,7 @@
         <v>0</v>
       </c>
       <c r="BO63" t="n">
-        <v>0.5179653167724609</v>
+        <v>0.6278612613677979</v>
       </c>
     </row>
     <row r="64">
@@ -14685,7 +14685,7 @@
         <v>0</v>
       </c>
       <c r="BO64" t="n">
-        <v>0.6165452003479004</v>
+        <v>0.6266006827354431</v>
       </c>
     </row>
     <row r="65">
@@ -14906,7 +14906,7 @@
         <v>0</v>
       </c>
       <c r="BO65" t="n">
-        <v>0.7385632991790771</v>
+        <v>0.7793653011322021</v>
       </c>
     </row>
     <row r="66">
@@ -15127,7 +15127,7 @@
         <v>0.073</v>
       </c>
       <c r="BO66" t="n">
-        <v>0.1064202636480331</v>
+        <v>0.2175709456205368</v>
       </c>
     </row>
     <row r="67">
@@ -15348,7 +15348,7 @@
         <v>0</v>
       </c>
       <c r="BO67" t="n">
-        <v>0.6184762716293335</v>
+        <v>0.5856631398200989</v>
       </c>
     </row>
     <row r="68">
@@ -15569,7 +15569,7 @@
         <v>0</v>
       </c>
       <c r="BO68" t="n">
-        <v>0.1669981777667999</v>
+        <v>0.2039490342140198</v>
       </c>
     </row>
     <row r="69">
@@ -15790,7 +15790,7 @@
         <v>0</v>
       </c>
       <c r="BO69" t="n">
-        <v>0.8024246096611023</v>
+        <v>0.698826014995575</v>
       </c>
     </row>
     <row r="70">
@@ -16011,7 +16011,7 @@
         <v>0</v>
       </c>
       <c r="BO70" t="n">
-        <v>0.7501640915870667</v>
+        <v>0.7884714603424072</v>
       </c>
     </row>
     <row r="71">
@@ -16232,7 +16232,7 @@
         <v>0</v>
       </c>
       <c r="BO71" t="n">
-        <v>0.4482934474945068</v>
+        <v>0.157875120639801</v>
       </c>
     </row>
     <row r="72">
@@ -16453,7 +16453,7 @@
         <v>0</v>
       </c>
       <c r="BO72" t="n">
-        <v>0.6727988123893738</v>
+        <v>0.7256271243095398</v>
       </c>
     </row>
     <row r="73">
@@ -16674,7 +16674,7 @@
         <v>0</v>
       </c>
       <c r="BO73" t="n">
-        <v>0.6912818551063538</v>
+        <v>0.7218974232673645</v>
       </c>
     </row>
     <row r="74">
@@ -16895,7 +16895,7 @@
         <v>0</v>
       </c>
       <c r="BO74" t="n">
-        <v>0.7438215613365173</v>
+        <v>0.7109302878379822</v>
       </c>
     </row>
     <row r="75">
@@ -17116,7 +17116,7 @@
         <v>0</v>
       </c>
       <c r="BO75" t="n">
-        <v>0.7334622144699097</v>
+        <v>0.7295388579368591</v>
       </c>
     </row>
     <row r="76">
@@ -17337,7 +17337,7 @@
         <v>0</v>
       </c>
       <c r="BO76" t="n">
-        <v>0.6867191791534424</v>
+        <v>0.6587293744087219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>